<commit_message>
Burdown chart sprint 1
</commit_message>
<xml_diff>
--- a/Visualisation de l'avancée.xlsx
+++ b/Visualisation de l'avancée.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAMP\htdocs\sae_web_s1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682478DB-B2D6-4488-9A98-AAA1ACEE19F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB9637E-DF66-4314-BEAF-957AE6A27EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1DBFED6A-AD0D-4074-98D6-F50E930B30CF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Point d'effort :</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>vendredi 13</t>
+  </si>
+  <si>
+    <t>Rendu</t>
   </si>
 </sst>
 </file>
@@ -360,7 +363,16 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1560,7 +1572,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1720,7 +1732,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
@@ -1730,15 +1742,27 @@
       <c r="A20">
         <v>19</v>
       </c>
+      <c r="B20">
+        <v>13</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>